<commit_message>
passing total price to checkout page
</commit_message>
<xml_diff>
--- a/xlsx/RedressRoutes.xlsx
+++ b/xlsx/RedressRoutes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Desktop\redress_web_integrator1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Desktop\redress_web_integrator1\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAEED4E-BD57-4235-8D44-E6AF3E4D38E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F659E9-9889-4C73-88E0-C70040B62573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E3F4C942-C68E-4534-8EE5-F2EB000981AE}"/>
+    <workbookView xWindow="20370" yWindow="-4860" windowWidth="29040" windowHeight="15990" xr2:uid="{E3F4C942-C68E-4534-8EE5-F2EB000981AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -273,7 +273,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -297,26 +297,26 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,10 +699,10 @@
   <dimension ref="B2:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G26:G27"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -718,7 +718,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
         <v>0</v>
@@ -746,19 +746,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6">
-        <v>13100484</v>
+        <v>13100488</v>
       </c>
       <c r="D3" s="7" t="str">
         <f>_xlfn.WEBSERVICE("https://viacep.com.br/ws/" &amp; C3 &amp; "/xml/")</f>
         <v>&lt;?xml version="1.0" encoding="UTF-8"?&gt;
 &lt;xmlcep&gt;
-  &lt;cep&gt;13100-484&lt;/cep&gt;
-  &lt;logradouro&gt;Rua João Ramalho&lt;/logradouro&gt;
+  &lt;cep&gt;13100-488&lt;/cep&gt;
+  &lt;logradouro&gt;Rua Otávio Tisseli Filho&lt;/logradouro&gt;
   &lt;complemento&gt;&lt;/complemento&gt;
   &lt;bairro&gt;Vila Lemos&lt;/bairro&gt;
   &lt;localidade&gt;Campinas&lt;/localidade&gt;
@@ -783,7 +783,7 @@
       </c>
       <c r="H3" s="5" t="str" cm="1">
         <f t="array" ref="H3">_xlfn.FILTERXML(D3,"//xmlcep/logradouro")</f>
-        <v>Rua João Ramalho</v>
+        <v>Rua Otávio Tisseli Filho</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>13</v>
@@ -797,7 +797,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
@@ -881,7 +881,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -926,28 +926,28 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -955,63 +955,63 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
     </row>
-    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
     </row>
-    <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
       <c r="O14" s="9"/>
     </row>
-    <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="17" t="s">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C21" s="13" t="str" cm="1">
         <f t="array" ref="C21">_xlfn.FILTERXML(D3,"//xmlcep/localidade") &amp; ", " &amp; _xlfn.FILTERXML(D3,"//xmlcep/uf") &amp; ", " &amp;  "Brasil"</f>
         <v>Campinas, SP, Brasil</v>
@@ -1024,38 +1024,38 @@
         <f t="array" ref="E21:E22">_xlfn.FILTERXML(K4,"DistanceMatrixResponse/row/element/duration/text")</f>
         <v>1 day 2 hours</v>
       </c>
-      <c r="F21" s="14" t="str" cm="1">
+      <c r="F21" s="19" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.FILTERXML(D5,"//xmlcep/localidade") &amp; ", " &amp; _xlfn.FILTERXML(D5,"//xmlcep/uf") &amp; ", " &amp;  "Brasil"</f>
         <v>Feira de Santana, BA, Brasil</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="4"/>
       <c r="C22" s="13" t="str" cm="1">
         <f t="array" ref="C22">_xlfn.FILTERXML(D4,"//xmlcep/localidade") &amp; ", " &amp; _xlfn.FILTERXML(D4,"//xmlcep/uf") &amp; ", " &amp;  "Brasil"</f>
         <v>Valinhos, SP, Brasil</v>
       </c>
-      <c r="D22" s="16" t="str">
+      <c r="D22" s="14" t="str">
         <v>1,838 km</v>
       </c>
       <c r="E22" s="13" t="str">
         <v>1 day 2 hours</v>
       </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E23" s="19" t="s">
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E23" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E24" s="20" cm="1">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="18" cm="1">
         <f t="array" ref="E24:E25">_xlfn.FILTERXML(K4,"DistanceMatrixResponse/row/element/duration/value") / 3600</f>
         <v>25.668055555555554</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E25" s="20">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E25" s="18">
         <v>25.587777777777777</v>
       </c>
     </row>

</xml_diff>